<commit_message>
fix: prevent hidden columns from being labeled upon detecting changes (#11)
* Skip hidden columns when searching for changes within rows

* Regenerate merged AHB files
</commit_message>
<xml_diff>
--- a/data/output/FV2304_FV2210/INVOIC/31001.xlsx
+++ b/data/output/FV2304_FV2210/INVOIC/31001.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4283" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4139" uniqueCount="476">
   <si>
     <t>#</t>
   </si>
@@ -6896,48 +6896,46 @@
       <c r="V105" s="11"/>
     </row>
     <row r="106" spans="1:22">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C106" s="5" t="s">
+      <c r="C106" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="D106" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
-      <c r="H106" s="5"/>
-      <c r="I106" s="5"/>
-      <c r="J106" s="5" t="s">
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K106" s="5"/>
-      <c r="L106" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M106" s="5" t="s">
+      <c r="K106" s="2"/>
+      <c r="L106" s="4"/>
+      <c r="M106" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N106" s="5" t="s">
+      <c r="N106" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O106" s="5" t="s">
+      <c r="O106" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P106" s="5"/>
-      <c r="Q106" s="5"/>
-      <c r="R106" s="5"/>
-      <c r="S106" s="5"/>
-      <c r="T106" s="5"/>
-      <c r="U106" s="5" t="s">
+      <c r="P106" s="2"/>
+      <c r="Q106" s="2"/>
+      <c r="R106" s="2"/>
+      <c r="S106" s="2"/>
+      <c r="T106" s="2"/>
+      <c r="U106" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V106" s="5"/>
+      <c r="V106" s="2"/>
     </row>
     <row r="107" spans="1:22">
       <c r="A107" s="5" t="s">
@@ -6967,9 +6965,7 @@
         <v>260</v>
       </c>
       <c r="K107" s="5"/>
-      <c r="L107" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L107" s="4"/>
       <c r="M107" s="5" t="s">
         <v>37</v>
       </c>
@@ -7023,9 +7019,7 @@
       <c r="K108" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="L108" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L108" s="4"/>
       <c r="M108" s="5" t="s">
         <v>37</v>
       </c>
@@ -7052,44 +7046,42 @@
       </c>
     </row>
     <row r="109" spans="1:22">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C109" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="5"/>
-      <c r="G109" s="5"/>
-      <c r="H109" s="5"/>
-      <c r="I109" s="5"/>
-      <c r="J109" s="5" t="s">
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K109" s="5"/>
-      <c r="L109" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M109" s="5" t="s">
+      <c r="K109" s="2"/>
+      <c r="L109" s="4"/>
+      <c r="M109" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N109" s="5" t="s">
+      <c r="N109" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O109" s="5"/>
-      <c r="P109" s="5"/>
-      <c r="Q109" s="5"/>
-      <c r="R109" s="5"/>
-      <c r="S109" s="5"/>
-      <c r="T109" s="5"/>
-      <c r="U109" s="5" t="s">
+      <c r="O109" s="2"/>
+      <c r="P109" s="2"/>
+      <c r="Q109" s="2"/>
+      <c r="R109" s="2"/>
+      <c r="S109" s="2"/>
+      <c r="T109" s="2"/>
+      <c r="U109" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V109" s="5"/>
+      <c r="V109" s="2"/>
     </row>
     <row r="110" spans="1:22">
       <c r="A110" s="5" t="s">
@@ -7113,9 +7105,7 @@
         <v>259</v>
       </c>
       <c r="K110" s="5"/>
-      <c r="L110" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L110" s="4"/>
       <c r="M110" s="5" t="s">
         <v>38</v>
       </c>
@@ -7163,9 +7153,7 @@
         <v>260</v>
       </c>
       <c r="K111" s="5"/>
-      <c r="L111" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L111" s="4"/>
       <c r="M111" s="5" t="s">
         <v>38</v>
       </c>
@@ -7219,9 +7207,7 @@
         <v>260</v>
       </c>
       <c r="K112" s="5"/>
-      <c r="L112" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L112" s="4"/>
       <c r="M112" s="5" t="s">
         <v>38</v>
       </c>
@@ -7275,9 +7261,7 @@
         <v>260</v>
       </c>
       <c r="K113" s="5"/>
-      <c r="L113" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L113" s="4"/>
       <c r="M113" s="5" t="s">
         <v>38</v>
       </c>
@@ -7304,44 +7288,42 @@
       <c r="V113" s="5"/>
     </row>
     <row r="114" spans="1:22">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B114" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C114" s="5" t="s">
+      <c r="C114" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D114" s="5"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
-      <c r="G114" s="5"/>
-      <c r="H114" s="5"/>
-      <c r="I114" s="5"/>
-      <c r="J114" s="5" t="s">
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K114" s="5"/>
-      <c r="L114" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M114" s="5" t="s">
+      <c r="K114" s="2"/>
+      <c r="L114" s="4"/>
+      <c r="M114" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N114" s="5" t="s">
+      <c r="N114" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="O114" s="5"/>
-      <c r="P114" s="5"/>
-      <c r="Q114" s="5"/>
-      <c r="R114" s="5"/>
-      <c r="S114" s="5"/>
-      <c r="T114" s="5"/>
-      <c r="U114" s="5" t="s">
+      <c r="O114" s="2"/>
+      <c r="P114" s="2"/>
+      <c r="Q114" s="2"/>
+      <c r="R114" s="2"/>
+      <c r="S114" s="2"/>
+      <c r="T114" s="2"/>
+      <c r="U114" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V114" s="5"/>
+      <c r="V114" s="2"/>
     </row>
     <row r="115" spans="1:22">
       <c r="A115" s="5" t="s">
@@ -7365,9 +7347,7 @@
         <v>259</v>
       </c>
       <c r="K115" s="5"/>
-      <c r="L115" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L115" s="4"/>
       <c r="M115" s="5" t="s">
         <v>39</v>
       </c>
@@ -7415,9 +7395,7 @@
         <v>260</v>
       </c>
       <c r="K116" s="5"/>
-      <c r="L116" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L116" s="4"/>
       <c r="M116" s="5" t="s">
         <v>39</v>
       </c>
@@ -7444,48 +7422,46 @@
       <c r="V116" s="5"/>
     </row>
     <row r="117" spans="1:22">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B117" s="5" t="s">
+      <c r="B117" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C117" s="5" t="s">
+      <c r="C117" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="D117" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
-      <c r="H117" s="5"/>
-      <c r="I117" s="5"/>
-      <c r="J117" s="5" t="s">
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K117" s="5"/>
-      <c r="L117" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M117" s="5" t="s">
+      <c r="K117" s="2"/>
+      <c r="L117" s="4"/>
+      <c r="M117" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N117" s="5" t="s">
+      <c r="N117" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="O117" s="5" t="s">
+      <c r="O117" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="P117" s="5"/>
-      <c r="Q117" s="5"/>
-      <c r="R117" s="5"/>
-      <c r="S117" s="5"/>
-      <c r="T117" s="5"/>
-      <c r="U117" s="5" t="s">
+      <c r="P117" s="2"/>
+      <c r="Q117" s="2"/>
+      <c r="R117" s="2"/>
+      <c r="S117" s="2"/>
+      <c r="T117" s="2"/>
+      <c r="U117" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V117" s="5"/>
+      <c r="V117" s="2"/>
     </row>
     <row r="118" spans="1:22">
       <c r="A118" s="5" t="s">
@@ -7515,9 +7491,7 @@
         <v>260</v>
       </c>
       <c r="K118" s="5"/>
-      <c r="L118" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L118" s="4"/>
       <c r="M118" s="5" t="s">
         <v>40</v>
       </c>
@@ -7627,9 +7601,7 @@
         <v>260</v>
       </c>
       <c r="K120" s="5"/>
-      <c r="L120" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L120" s="4"/>
       <c r="M120" s="5" t="s">
         <v>40</v>
       </c>
@@ -7656,44 +7628,42 @@
       <c r="V120" s="5"/>
     </row>
     <row r="121" spans="1:22">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B121" s="5" t="s">
+      <c r="B121" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C121" s="5" t="s">
+      <c r="C121" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
-      <c r="H121" s="5"/>
-      <c r="I121" s="5"/>
-      <c r="J121" s="5" t="s">
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K121" s="5"/>
-      <c r="L121" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M121" s="5" t="s">
+      <c r="K121" s="2"/>
+      <c r="L121" s="4"/>
+      <c r="M121" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N121" s="5" t="s">
+      <c r="N121" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="O121" s="5"/>
-      <c r="P121" s="5"/>
-      <c r="Q121" s="5"/>
-      <c r="R121" s="5"/>
-      <c r="S121" s="5"/>
-      <c r="T121" s="5"/>
-      <c r="U121" s="5" t="s">
+      <c r="O121" s="2"/>
+      <c r="P121" s="2"/>
+      <c r="Q121" s="2"/>
+      <c r="R121" s="2"/>
+      <c r="S121" s="2"/>
+      <c r="T121" s="2"/>
+      <c r="U121" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V121" s="5"/>
+      <c r="V121" s="2"/>
     </row>
     <row r="122" spans="1:22">
       <c r="A122" s="5" t="s">
@@ -7717,9 +7687,7 @@
         <v>259</v>
       </c>
       <c r="K122" s="5"/>
-      <c r="L122" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L122" s="4"/>
       <c r="M122" s="5" t="s">
         <v>41</v>
       </c>
@@ -7767,9 +7735,7 @@
       <c r="K123" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="L123" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L123" s="4"/>
       <c r="M123" s="5" t="s">
         <v>41</v>
       </c>
@@ -7823,9 +7789,7 @@
       <c r="K124" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="L124" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L124" s="4"/>
       <c r="M124" s="5" t="s">
         <v>41</v>
       </c>
@@ -7879,9 +7843,7 @@
         <v>260</v>
       </c>
       <c r="K125" s="5"/>
-      <c r="L125" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L125" s="4"/>
       <c r="M125" s="5" t="s">
         <v>41</v>
       </c>
@@ -7908,48 +7870,46 @@
       <c r="V125" s="5"/>
     </row>
     <row r="126" spans="1:22">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B126" s="5" t="s">
+      <c r="B126" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C126" s="5" t="s">
+      <c r="C126" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D126" s="5" t="s">
+      <c r="D126" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E126" s="5"/>
-      <c r="F126" s="5"/>
-      <c r="G126" s="5"/>
-      <c r="H126" s="5"/>
-      <c r="I126" s="5"/>
-      <c r="J126" s="5" t="s">
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+      <c r="J126" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K126" s="5"/>
-      <c r="L126" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M126" s="5" t="s">
+      <c r="K126" s="2"/>
+      <c r="L126" s="4"/>
+      <c r="M126" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N126" s="5" t="s">
+      <c r="N126" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="O126" s="5" t="s">
+      <c r="O126" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="P126" s="5"/>
-      <c r="Q126" s="5"/>
-      <c r="R126" s="5"/>
-      <c r="S126" s="5"/>
-      <c r="T126" s="5"/>
-      <c r="U126" s="5" t="s">
+      <c r="P126" s="2"/>
+      <c r="Q126" s="2"/>
+      <c r="R126" s="2"/>
+      <c r="S126" s="2"/>
+      <c r="T126" s="2"/>
+      <c r="U126" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V126" s="5"/>
+      <c r="V126" s="2"/>
     </row>
     <row r="127" spans="1:22">
       <c r="A127" s="5" t="s">
@@ -7979,9 +7939,7 @@
         <v>260</v>
       </c>
       <c r="K127" s="5"/>
-      <c r="L127" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L127" s="4"/>
       <c r="M127" s="5" t="s">
         <v>42</v>
       </c>
@@ -8035,9 +7993,7 @@
       <c r="K128" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="L128" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L128" s="4"/>
       <c r="M128" s="5" t="s">
         <v>42</v>
       </c>
@@ -8124,50 +8080,48 @@
       </c>
     </row>
     <row r="130" spans="1:22">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="C130" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D130" s="5" t="s">
+      <c r="D130" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E130" s="5"/>
-      <c r="F130" s="5"/>
-      <c r="G130" s="5"/>
-      <c r="H130" s="5"/>
-      <c r="I130" s="5"/>
-      <c r="J130" s="5" t="s">
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
+      <c r="J130" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K130" s="5" t="s">
+      <c r="K130" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="L130" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M130" s="5" t="s">
+      <c r="L130" s="4"/>
+      <c r="M130" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N130" s="5" t="s">
+      <c r="N130" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="O130" s="5" t="s">
+      <c r="O130" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="P130" s="5"/>
-      <c r="Q130" s="5"/>
-      <c r="R130" s="5"/>
-      <c r="S130" s="5"/>
-      <c r="T130" s="5"/>
-      <c r="U130" s="5" t="s">
+      <c r="P130" s="2"/>
+      <c r="Q130" s="2"/>
+      <c r="R130" s="2"/>
+      <c r="S130" s="2"/>
+      <c r="T130" s="2"/>
+      <c r="U130" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V130" s="5" t="s">
+      <c r="V130" s="2" t="s">
         <v>292</v>
       </c>
     </row>
@@ -8199,9 +8153,7 @@
         <v>260</v>
       </c>
       <c r="K131" s="5"/>
-      <c r="L131" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L131" s="4"/>
       <c r="M131" s="5" t="s">
         <v>43</v>
       </c>
@@ -8253,9 +8205,7 @@
         <v>262</v>
       </c>
       <c r="K132" s="5"/>
-      <c r="L132" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L132" s="4"/>
       <c r="M132" s="5" t="s">
         <v>43</v>
       </c>
@@ -8307,9 +8257,7 @@
         <v>260</v>
       </c>
       <c r="K133" s="5"/>
-      <c r="L133" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L133" s="4"/>
       <c r="M133" s="5" t="s">
         <v>43</v>
       </c>
@@ -8336,50 +8284,48 @@
       <c r="V133" s="5"/>
     </row>
     <row r="134" spans="1:22">
-      <c r="A134" s="5" t="s">
+      <c r="A134" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B134" s="5" t="s">
+      <c r="B134" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C134" s="5" t="s">
+      <c r="C134" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D134" s="5" t="s">
+      <c r="D134" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E134" s="5"/>
-      <c r="F134" s="5"/>
-      <c r="G134" s="5"/>
-      <c r="H134" s="5"/>
-      <c r="I134" s="5"/>
-      <c r="J134" s="5" t="s">
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+      <c r="J134" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K134" s="5" t="s">
+      <c r="K134" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="L134" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M134" s="5" t="s">
+      <c r="L134" s="4"/>
+      <c r="M134" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N134" s="5" t="s">
+      <c r="N134" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="O134" s="5" t="s">
+      <c r="O134" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="P134" s="5"/>
-      <c r="Q134" s="5"/>
-      <c r="R134" s="5"/>
-      <c r="S134" s="5"/>
-      <c r="T134" s="5"/>
-      <c r="U134" s="5" t="s">
+      <c r="P134" s="2"/>
+      <c r="Q134" s="2"/>
+      <c r="R134" s="2"/>
+      <c r="S134" s="2"/>
+      <c r="T134" s="2"/>
+      <c r="U134" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V134" s="5" t="s">
+      <c r="V134" s="2" t="s">
         <v>292</v>
       </c>
     </row>
@@ -8411,9 +8357,7 @@
         <v>260</v>
       </c>
       <c r="K135" s="5"/>
-      <c r="L135" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L135" s="4"/>
       <c r="M135" s="5" t="s">
         <v>44</v>
       </c>
@@ -8465,9 +8409,7 @@
         <v>262</v>
       </c>
       <c r="K136" s="5"/>
-      <c r="L136" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L136" s="4"/>
       <c r="M136" s="5" t="s">
         <v>44</v>
       </c>
@@ -8519,9 +8461,7 @@
         <v>260</v>
       </c>
       <c r="K137" s="5"/>
-      <c r="L137" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L137" s="4"/>
       <c r="M137" s="5" t="s">
         <v>44</v>
       </c>
@@ -8548,44 +8488,42 @@
       <c r="V137" s="5"/>
     </row>
     <row r="138" spans="1:22">
-      <c r="A138" s="5" t="s">
+      <c r="A138" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B138" s="5" t="s">
+      <c r="B138" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C138" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D138" s="5"/>
-      <c r="E138" s="5"/>
-      <c r="F138" s="5"/>
-      <c r="G138" s="5"/>
-      <c r="H138" s="5"/>
-      <c r="I138" s="5"/>
-      <c r="J138" s="5" t="s">
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
+      <c r="J138" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K138" s="5"/>
-      <c r="L138" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M138" s="5" t="s">
+      <c r="K138" s="2"/>
+      <c r="L138" s="4"/>
+      <c r="M138" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N138" s="5" t="s">
+      <c r="N138" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="O138" s="5"/>
-      <c r="P138" s="5"/>
-      <c r="Q138" s="5"/>
-      <c r="R138" s="5"/>
-      <c r="S138" s="5"/>
-      <c r="T138" s="5"/>
-      <c r="U138" s="5" t="s">
+      <c r="O138" s="2"/>
+      <c r="P138" s="2"/>
+      <c r="Q138" s="2"/>
+      <c r="R138" s="2"/>
+      <c r="S138" s="2"/>
+      <c r="T138" s="2"/>
+      <c r="U138" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V138" s="5"/>
+      <c r="V138" s="2"/>
     </row>
     <row r="139" spans="1:22">
       <c r="A139" s="5" t="s">
@@ -8609,9 +8547,7 @@
         <v>259</v>
       </c>
       <c r="K139" s="5"/>
-      <c r="L139" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L139" s="4"/>
       <c r="M139" s="5" t="s">
         <v>45</v>
       </c>
@@ -8659,9 +8595,7 @@
         <v>260</v>
       </c>
       <c r="K140" s="5"/>
-      <c r="L140" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L140" s="4"/>
       <c r="M140" s="5" t="s">
         <v>45</v>
       </c>
@@ -8715,9 +8649,7 @@
       <c r="K141" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="L141" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L141" s="4"/>
       <c r="M141" s="5" t="s">
         <v>45</v>
       </c>
@@ -8744,44 +8676,42 @@
       </c>
     </row>
     <row r="142" spans="1:22">
-      <c r="A142" s="5" t="s">
+      <c r="A142" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B142" s="5" t="s">
+      <c r="B142" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C142" s="5" t="s">
+      <c r="C142" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D142" s="5"/>
-      <c r="E142" s="5"/>
-      <c r="F142" s="5"/>
-      <c r="G142" s="5"/>
-      <c r="H142" s="5"/>
-      <c r="I142" s="5"/>
-      <c r="J142" s="5" t="s">
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
+      <c r="J142" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K142" s="5"/>
-      <c r="L142" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M142" s="5" t="s">
+      <c r="K142" s="2"/>
+      <c r="L142" s="4"/>
+      <c r="M142" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="N142" s="5" t="s">
+      <c r="N142" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="O142" s="5"/>
-      <c r="P142" s="5"/>
-      <c r="Q142" s="5"/>
-      <c r="R142" s="5"/>
-      <c r="S142" s="5"/>
-      <c r="T142" s="5"/>
-      <c r="U142" s="5" t="s">
+      <c r="O142" s="2"/>
+      <c r="P142" s="2"/>
+      <c r="Q142" s="2"/>
+      <c r="R142" s="2"/>
+      <c r="S142" s="2"/>
+      <c r="T142" s="2"/>
+      <c r="U142" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V142" s="5"/>
+      <c r="V142" s="2"/>
     </row>
     <row r="143" spans="1:22">
       <c r="A143" s="5" t="s">
@@ -8805,9 +8735,7 @@
         <v>259</v>
       </c>
       <c r="K143" s="5"/>
-      <c r="L143" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L143" s="4"/>
       <c r="M143" s="5" t="s">
         <v>46</v>
       </c>
@@ -8855,9 +8783,7 @@
         <v>260</v>
       </c>
       <c r="K144" s="5"/>
-      <c r="L144" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L144" s="4"/>
       <c r="M144" s="5" t="s">
         <v>46</v>
       </c>
@@ -8911,9 +8837,7 @@
       <c r="K145" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="L145" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L145" s="4"/>
       <c r="M145" s="5" t="s">
         <v>46</v>
       </c>
@@ -8940,44 +8864,42 @@
       </c>
     </row>
     <row r="146" spans="1:22">
-      <c r="A146" s="5" t="s">
+      <c r="A146" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B146" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C146" s="5" t="s">
+      <c r="C146" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D146" s="5"/>
-      <c r="E146" s="5"/>
-      <c r="F146" s="5"/>
-      <c r="G146" s="5"/>
-      <c r="H146" s="5"/>
-      <c r="I146" s="5"/>
-      <c r="J146" s="5" t="s">
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K146" s="5"/>
-      <c r="L146" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M146" s="5" t="s">
+      <c r="K146" s="2"/>
+      <c r="L146" s="4"/>
+      <c r="M146" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="N146" s="5" t="s">
+      <c r="N146" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O146" s="5"/>
-      <c r="P146" s="5"/>
-      <c r="Q146" s="5"/>
-      <c r="R146" s="5"/>
-      <c r="S146" s="5"/>
-      <c r="T146" s="5"/>
-      <c r="U146" s="5" t="s">
+      <c r="O146" s="2"/>
+      <c r="P146" s="2"/>
+      <c r="Q146" s="2"/>
+      <c r="R146" s="2"/>
+      <c r="S146" s="2"/>
+      <c r="T146" s="2"/>
+      <c r="U146" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V146" s="5"/>
+      <c r="V146" s="2"/>
     </row>
     <row r="147" spans="1:22">
       <c r="A147" s="5" t="s">
@@ -9001,9 +8923,7 @@
         <v>259</v>
       </c>
       <c r="K147" s="5"/>
-      <c r="L147" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L147" s="4"/>
       <c r="M147" s="5" t="s">
         <v>47</v>
       </c>
@@ -9051,9 +8971,7 @@
         <v>260</v>
       </c>
       <c r="K148" s="5"/>
-      <c r="L148" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L148" s="4"/>
       <c r="M148" s="5" t="s">
         <v>47</v>
       </c>
@@ -9107,9 +9025,7 @@
         <v>260</v>
       </c>
       <c r="K149" s="5"/>
-      <c r="L149" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L149" s="4"/>
       <c r="M149" s="5" t="s">
         <v>47</v>
       </c>
@@ -9163,9 +9079,7 @@
       <c r="K150" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="L150" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L150" s="4"/>
       <c r="M150" s="5" t="s">
         <v>47</v>
       </c>
@@ -9219,9 +9133,7 @@
         <v>260</v>
       </c>
       <c r="K151" s="5"/>
-      <c r="L151" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L151" s="4"/>
       <c r="M151" s="5" t="s">
         <v>47</v>
       </c>
@@ -9275,9 +9187,7 @@
         <v>260</v>
       </c>
       <c r="K152" s="5"/>
-      <c r="L152" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L152" s="4"/>
       <c r="M152" s="5" t="s">
         <v>47</v>
       </c>
@@ -9331,9 +9241,7 @@
         <v>260</v>
       </c>
       <c r="K153" s="5"/>
-      <c r="L153" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L153" s="4"/>
       <c r="M153" s="5" t="s">
         <v>47</v>
       </c>
@@ -9360,44 +9268,42 @@
       <c r="V153" s="5"/>
     </row>
     <row r="154" spans="1:22">
-      <c r="A154" s="5" t="s">
+      <c r="A154" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C154" s="5"/>
-      <c r="D154" s="5" t="s">
+      <c r="C154" s="2"/>
+      <c r="D154" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E154" s="5"/>
-      <c r="F154" s="5"/>
-      <c r="G154" s="5"/>
-      <c r="H154" s="5"/>
-      <c r="I154" s="5"/>
-      <c r="J154" s="5" t="s">
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+      <c r="J154" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K154" s="5"/>
-      <c r="L154" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M154" s="5" t="s">
+      <c r="K154" s="2"/>
+      <c r="L154" s="4"/>
+      <c r="M154" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="N154" s="5"/>
-      <c r="O154" s="5" t="s">
+      <c r="N154" s="2"/>
+      <c r="O154" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P154" s="5"/>
-      <c r="Q154" s="5"/>
-      <c r="R154" s="5"/>
-      <c r="S154" s="5"/>
-      <c r="T154" s="5"/>
-      <c r="U154" s="5" t="s">
+      <c r="P154" s="2"/>
+      <c r="Q154" s="2"/>
+      <c r="R154" s="2"/>
+      <c r="S154" s="2"/>
+      <c r="T154" s="2"/>
+      <c r="U154" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V154" s="5"/>
+      <c r="V154" s="2"/>
     </row>
     <row r="155" spans="1:22">
       <c r="A155" s="5" t="s">
@@ -9425,9 +9331,7 @@
         <v>260</v>
       </c>
       <c r="K155" s="5"/>
-      <c r="L155" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L155" s="4"/>
       <c r="M155" s="5" t="s">
         <v>48</v>
       </c>
@@ -9452,44 +9356,42 @@
       <c r="V155" s="5"/>
     </row>
     <row r="156" spans="1:22">
-      <c r="A156" s="5" t="s">
+      <c r="A156" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B156" s="5" t="s">
+      <c r="B156" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C156" s="5" t="s">
+      <c r="C156" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D156" s="5"/>
-      <c r="E156" s="5"/>
-      <c r="F156" s="5"/>
-      <c r="G156" s="5"/>
-      <c r="H156" s="5"/>
-      <c r="I156" s="5"/>
-      <c r="J156" s="5" t="s">
+      <c r="D156" s="2"/>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="2"/>
+      <c r="H156" s="2"/>
+      <c r="I156" s="2"/>
+      <c r="J156" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K156" s="5"/>
-      <c r="L156" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M156" s="5" t="s">
+      <c r="K156" s="2"/>
+      <c r="L156" s="4"/>
+      <c r="M156" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N156" s="5" t="s">
+      <c r="N156" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="O156" s="5"/>
-      <c r="P156" s="5"/>
-      <c r="Q156" s="5"/>
-      <c r="R156" s="5"/>
-      <c r="S156" s="5"/>
-      <c r="T156" s="5"/>
-      <c r="U156" s="5" t="s">
+      <c r="O156" s="2"/>
+      <c r="P156" s="2"/>
+      <c r="Q156" s="2"/>
+      <c r="R156" s="2"/>
+      <c r="S156" s="2"/>
+      <c r="T156" s="2"/>
+      <c r="U156" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V156" s="5"/>
+      <c r="V156" s="2"/>
     </row>
     <row r="157" spans="1:22">
       <c r="A157" s="5" t="s">
@@ -9513,9 +9415,7 @@
         <v>259</v>
       </c>
       <c r="K157" s="5"/>
-      <c r="L157" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L157" s="4"/>
       <c r="M157" s="5" t="s">
         <v>49</v>
       </c>
@@ -9563,9 +9463,7 @@
         <v>260</v>
       </c>
       <c r="K158" s="5"/>
-      <c r="L158" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L158" s="4"/>
       <c r="M158" s="5" t="s">
         <v>49</v>
       </c>
@@ -9619,9 +9517,7 @@
       <c r="K159" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="L159" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L159" s="4"/>
       <c r="M159" s="5" t="s">
         <v>49</v>
       </c>
@@ -9648,44 +9544,42 @@
       </c>
     </row>
     <row r="160" spans="1:22">
-      <c r="A160" s="5" t="s">
+      <c r="A160" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B160" s="5" t="s">
+      <c r="B160" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C160" s="5" t="s">
+      <c r="C160" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D160" s="5"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="5"/>
-      <c r="G160" s="5"/>
-      <c r="H160" s="5"/>
-      <c r="I160" s="5"/>
-      <c r="J160" s="5" t="s">
+      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
+      <c r="J160" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K160" s="5"/>
-      <c r="L160" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M160" s="5" t="s">
+      <c r="K160" s="2"/>
+      <c r="L160" s="4"/>
+      <c r="M160" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N160" s="5" t="s">
+      <c r="N160" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="O160" s="5"/>
-      <c r="P160" s="5"/>
-      <c r="Q160" s="5"/>
-      <c r="R160" s="5"/>
-      <c r="S160" s="5"/>
-      <c r="T160" s="5"/>
-      <c r="U160" s="5" t="s">
+      <c r="O160" s="2"/>
+      <c r="P160" s="2"/>
+      <c r="Q160" s="2"/>
+      <c r="R160" s="2"/>
+      <c r="S160" s="2"/>
+      <c r="T160" s="2"/>
+      <c r="U160" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V160" s="5"/>
+      <c r="V160" s="2"/>
     </row>
     <row r="161" spans="1:22">
       <c r="A161" s="5" t="s">
@@ -9709,9 +9603,7 @@
         <v>259</v>
       </c>
       <c r="K161" s="5"/>
-      <c r="L161" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L161" s="4"/>
       <c r="M161" s="5" t="s">
         <v>50</v>
       </c>
@@ -9759,9 +9651,7 @@
         <v>260</v>
       </c>
       <c r="K162" s="5"/>
-      <c r="L162" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L162" s="4"/>
       <c r="M162" s="5" t="s">
         <v>50</v>
       </c>
@@ -9815,9 +9705,7 @@
       <c r="K163" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="L163" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L163" s="4"/>
       <c r="M163" s="5" t="s">
         <v>50</v>
       </c>
@@ -9844,44 +9732,42 @@
       </c>
     </row>
     <row r="164" spans="1:22">
-      <c r="A164" s="5" t="s">
+      <c r="A164" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B164" s="5" t="s">
+      <c r="B164" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C164" s="5" t="s">
+      <c r="C164" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D164" s="5"/>
-      <c r="E164" s="5"/>
-      <c r="F164" s="5"/>
-      <c r="G164" s="5"/>
-      <c r="H164" s="5"/>
-      <c r="I164" s="5"/>
-      <c r="J164" s="5" t="s">
+      <c r="D164" s="2"/>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
+      <c r="G164" s="2"/>
+      <c r="H164" s="2"/>
+      <c r="I164" s="2"/>
+      <c r="J164" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K164" s="5"/>
-      <c r="L164" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M164" s="5" t="s">
+      <c r="K164" s="2"/>
+      <c r="L164" s="4"/>
+      <c r="M164" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N164" s="5" t="s">
+      <c r="N164" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O164" s="5"/>
-      <c r="P164" s="5"/>
-      <c r="Q164" s="5"/>
-      <c r="R164" s="5"/>
-      <c r="S164" s="5"/>
-      <c r="T164" s="5"/>
-      <c r="U164" s="5" t="s">
+      <c r="O164" s="2"/>
+      <c r="P164" s="2"/>
+      <c r="Q164" s="2"/>
+      <c r="R164" s="2"/>
+      <c r="S164" s="2"/>
+      <c r="T164" s="2"/>
+      <c r="U164" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V164" s="5"/>
+      <c r="V164" s="2"/>
     </row>
     <row r="165" spans="1:22">
       <c r="A165" s="5" t="s">
@@ -9905,9 +9791,7 @@
         <v>259</v>
       </c>
       <c r="K165" s="5"/>
-      <c r="L165" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L165" s="4"/>
       <c r="M165" s="5" t="s">
         <v>51</v>
       </c>
@@ -9955,9 +9839,7 @@
         <v>260</v>
       </c>
       <c r="K166" s="5"/>
-      <c r="L166" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L166" s="4"/>
       <c r="M166" s="5" t="s">
         <v>51</v>
       </c>
@@ -10011,9 +9893,7 @@
         <v>260</v>
       </c>
       <c r="K167" s="5"/>
-      <c r="L167" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L167" s="4"/>
       <c r="M167" s="5" t="s">
         <v>51</v>
       </c>
@@ -10067,9 +9947,7 @@
       <c r="K168" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="L168" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L168" s="4"/>
       <c r="M168" s="5" t="s">
         <v>51</v>
       </c>
@@ -10123,9 +10001,7 @@
         <v>260</v>
       </c>
       <c r="K169" s="5"/>
-      <c r="L169" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L169" s="4"/>
       <c r="M169" s="5" t="s">
         <v>51</v>
       </c>
@@ -10179,9 +10055,7 @@
         <v>260</v>
       </c>
       <c r="K170" s="5"/>
-      <c r="L170" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L170" s="4"/>
       <c r="M170" s="5" t="s">
         <v>51</v>
       </c>
@@ -10235,9 +10109,7 @@
         <v>260</v>
       </c>
       <c r="K171" s="5"/>
-      <c r="L171" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L171" s="4"/>
       <c r="M171" s="5" t="s">
         <v>51</v>
       </c>
@@ -10264,48 +10136,46 @@
       <c r="V171" s="5"/>
     </row>
     <row r="172" spans="1:22">
-      <c r="A172" s="5" t="s">
+      <c r="A172" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="B172" s="5" t="s">
+      <c r="B172" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C172" s="5" t="s">
+      <c r="C172" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D172" s="5" t="s">
+      <c r="D172" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E172" s="5"/>
-      <c r="F172" s="5"/>
-      <c r="G172" s="5"/>
-      <c r="H172" s="5"/>
-      <c r="I172" s="5"/>
-      <c r="J172" s="5" t="s">
+      <c r="E172" s="2"/>
+      <c r="F172" s="2"/>
+      <c r="G172" s="2"/>
+      <c r="H172" s="2"/>
+      <c r="I172" s="2"/>
+      <c r="J172" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K172" s="5"/>
-      <c r="L172" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M172" s="5" t="s">
+      <c r="K172" s="2"/>
+      <c r="L172" s="4"/>
+      <c r="M172" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N172" s="5" t="s">
+      <c r="N172" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O172" s="5" t="s">
+      <c r="O172" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="P172" s="5"/>
-      <c r="Q172" s="5"/>
-      <c r="R172" s="5"/>
-      <c r="S172" s="5"/>
-      <c r="T172" s="5"/>
-      <c r="U172" s="5" t="s">
+      <c r="P172" s="2"/>
+      <c r="Q172" s="2"/>
+      <c r="R172" s="2"/>
+      <c r="S172" s="2"/>
+      <c r="T172" s="2"/>
+      <c r="U172" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V172" s="5"/>
+      <c r="V172" s="2"/>
     </row>
     <row r="173" spans="1:22">
       <c r="A173" s="5" t="s">
@@ -10335,9 +10205,7 @@
         <v>260</v>
       </c>
       <c r="K173" s="5"/>
-      <c r="L173" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L173" s="4"/>
       <c r="M173" s="5" t="s">
         <v>52</v>
       </c>
@@ -10391,9 +10259,7 @@
       <c r="K174" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="L174" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L174" s="4"/>
       <c r="M174" s="5" t="s">
         <v>52</v>
       </c>
@@ -10420,48 +10286,46 @@
       </c>
     </row>
     <row r="175" spans="1:22">
-      <c r="A175" s="5" t="s">
+      <c r="A175" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="B175" s="5" t="s">
+      <c r="B175" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C175" s="5" t="s">
+      <c r="C175" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D175" s="5" t="s">
+      <c r="D175" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E175" s="5"/>
-      <c r="F175" s="5"/>
-      <c r="G175" s="5"/>
-      <c r="H175" s="5"/>
-      <c r="I175" s="5"/>
-      <c r="J175" s="5" t="s">
+      <c r="E175" s="2"/>
+      <c r="F175" s="2"/>
+      <c r="G175" s="2"/>
+      <c r="H175" s="2"/>
+      <c r="I175" s="2"/>
+      <c r="J175" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K175" s="5"/>
-      <c r="L175" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M175" s="5" t="s">
+      <c r="K175" s="2"/>
+      <c r="L175" s="4"/>
+      <c r="M175" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N175" s="5" t="s">
+      <c r="N175" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O175" s="5" t="s">
+      <c r="O175" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="P175" s="5"/>
-      <c r="Q175" s="5"/>
-      <c r="R175" s="5"/>
-      <c r="S175" s="5"/>
-      <c r="T175" s="5"/>
-      <c r="U175" s="5" t="s">
+      <c r="P175" s="2"/>
+      <c r="Q175" s="2"/>
+      <c r="R175" s="2"/>
+      <c r="S175" s="2"/>
+      <c r="T175" s="2"/>
+      <c r="U175" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V175" s="5"/>
+      <c r="V175" s="2"/>
     </row>
     <row r="176" spans="1:22">
       <c r="A176" s="5" t="s">
@@ -10491,9 +10355,7 @@
         <v>260</v>
       </c>
       <c r="K176" s="5"/>
-      <c r="L176" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L176" s="4"/>
       <c r="M176" s="5" t="s">
         <v>53</v>
       </c>
@@ -10547,9 +10409,7 @@
       <c r="K177" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="L177" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L177" s="4"/>
       <c r="M177" s="5" t="s">
         <v>53</v>
       </c>
@@ -10576,44 +10436,42 @@
       </c>
     </row>
     <row r="178" spans="1:22">
-      <c r="A178" s="5" t="s">
+      <c r="A178" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B178" s="5" t="s">
+      <c r="B178" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C178" s="5"/>
-      <c r="D178" s="5" t="s">
+      <c r="C178" s="2"/>
+      <c r="D178" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E178" s="5"/>
-      <c r="F178" s="5"/>
-      <c r="G178" s="5"/>
-      <c r="H178" s="5"/>
-      <c r="I178" s="5"/>
-      <c r="J178" s="5" t="s">
+      <c r="E178" s="2"/>
+      <c r="F178" s="2"/>
+      <c r="G178" s="2"/>
+      <c r="H178" s="2"/>
+      <c r="I178" s="2"/>
+      <c r="J178" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="K178" s="5"/>
-      <c r="L178" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M178" s="5" t="s">
+      <c r="K178" s="2"/>
+      <c r="L178" s="4"/>
+      <c r="M178" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N178" s="5"/>
-      <c r="O178" s="5" t="s">
+      <c r="N178" s="2"/>
+      <c r="O178" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="P178" s="5"/>
-      <c r="Q178" s="5"/>
-      <c r="R178" s="5"/>
-      <c r="S178" s="5"/>
-      <c r="T178" s="5"/>
-      <c r="U178" s="5" t="s">
+      <c r="P178" s="2"/>
+      <c r="Q178" s="2"/>
+      <c r="R178" s="2"/>
+      <c r="S178" s="2"/>
+      <c r="T178" s="2"/>
+      <c r="U178" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="V178" s="5"/>
+      <c r="V178" s="2"/>
     </row>
     <row r="179" spans="1:22">
       <c r="A179" s="5" t="s">
@@ -10639,9 +10497,7 @@
         <v>260</v>
       </c>
       <c r="K179" s="5"/>
-      <c r="L179" s="7" t="s">
-        <v>296</v>
-      </c>
+      <c r="L179" s="4"/>
       <c r="M179" s="5" t="s">
         <v>54</v>
       </c>

</xml_diff>